<commit_message>
Fixed onload Post bug
</commit_message>
<xml_diff>
--- a/serverFolder/TestCases.xlsx
+++ b/serverFolder/TestCases.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -54,6 +54,63 @@
   </si>
   <si>
     <t xml:space="preserve"> Administrator - Selecting preferred language on the web-portal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the administrator selects english as a new language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  the web-portal will show all text in english</t>
+  </si>
+  <si>
+    <t>Select English as preferred language</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the administrator selects french as a new language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  the web-portal will show all text in french</t>
+  </si>
+  <si>
+    <t>Select French as preferred language</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the administrator selects swedish as a new language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  the web-portal will show all text in swedish</t>
+  </si>
+  <si>
+    <t>Select Swedish as preferred language</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> in order to keep track of the restaurant owners an administrator should be able to manage the restaurant owners  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the administrator is logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the administrator deletes an existing restaurant owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the restaurant owner should be deleted</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the restaurant information should be deleted</t>
+  </si>
+  <si>
+    <t>Delete an existing restaurant owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Manage restaurant owners</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the administrator creates a new restaurant owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the new restaurant owner should be added</t>
+  </si>
+  <si>
+    <t>Add a new restaurant owner</t>
   </si>
 </sst>
 </file>
@@ -108,7 +165,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -117,7 +174,7 @@
     <col min="1" max="1" width="8.25390625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="14.65625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="6.546875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="50.42578125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="50.44921875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="109.90625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -199,10 +256,336 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="B28:B32"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>